<commit_message>
updated for all hex values. Note invalid reg section is error prone
</commit_message>
<xml_diff>
--- a/Raw Data/OP Code Datasheet.xlsx
+++ b/Raw Data/OP Code Datasheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
   <si>
     <t>OP MODE</t>
   </si>
@@ -24,9 +24,6 @@
     <t>VALUE</t>
   </si>
   <si>
-    <t>100111001110101</t>
-  </si>
-  <si>
     <t>0100111001110101</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
     <t>01100000XXXXXX</t>
   </si>
   <si>
-    <t>0100111010XXXXX</t>
-  </si>
-  <si>
     <t>&gt;16</t>
   </si>
   <si>
@@ -274,6 +268,36 @@
   </si>
   <si>
     <t>81C0</t>
+  </si>
+  <si>
+    <t>41C0</t>
+  </si>
+  <si>
+    <t>8000</t>
+  </si>
+  <si>
+    <t>B000</t>
+  </si>
+  <si>
+    <t>E008</t>
+  </si>
+  <si>
+    <t>E018</t>
+  </si>
+  <si>
+    <t>E000</t>
+  </si>
+  <si>
+    <t>0180</t>
+  </si>
+  <si>
+    <t>0C00</t>
+  </si>
+  <si>
+    <t>0100111010XXXXXX</t>
+  </si>
+  <si>
+    <t>4E80</t>
   </si>
 </sst>
 </file>
@@ -309,11 +333,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,30 +676,30 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -671,171 +707,171 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4">
         <v>9</v>
       </c>
       <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
       <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6">
         <v>9</v>
       </c>
       <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="G6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>9</v>
       </c>
       <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D9">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -844,18 +880,18 @@
         <v>111</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -864,86 +900,95 @@
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -952,18 +997,21 @@
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4400</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -972,38 +1020,44 @@
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -1012,18 +1066,21 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1032,18 +1089,21 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -1052,69 +1112,79 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>90</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
         <v>67</v>
       </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>76</v>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="D25">
         <v>4</v>
@@ -1123,90 +1193,102 @@
         <v>11</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="C26" s="5">
+        <v>6000</v>
       </c>
       <c r="D26">
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="C27" s="5">
+        <v>6000</v>
       </c>
       <c r="D27">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>75</v>
+        <v>92</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="D28">
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C29" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="D29">
         <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separated code into separate files for sanities sake
</commit_message>
<xml_diff>
--- a/Raw Data/OP Code Datasheet.xlsx
+++ b/Raw Data/OP Code Datasheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="104">
   <si>
     <t>OP MODE</t>
   </si>
@@ -105,9 +105,6 @@
     <t>00XXXXXXXXXXXXXX</t>
   </si>
   <si>
-    <t>00 invalid size</t>
-  </si>
-  <si>
     <t>Invalid sizes</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>1011XXXXXXXXXXXX</t>
   </si>
   <si>
-    <t>000,111</t>
-  </si>
-  <si>
     <t>1110XXXDSSR01XXX</t>
   </si>
   <si>
@@ -298,6 +292,42 @@
   </si>
   <si>
     <t>4E80</t>
+  </si>
+  <si>
+    <t>111,'101,'100,'110,'</t>
+  </si>
+  <si>
+    <t>000,111,'001,'010</t>
+  </si>
+  <si>
+    <t>OP CODE</t>
+  </si>
+  <si>
+    <t>ORDER OF OPERATIONS</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>EOR/CMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR </t>
+  </si>
+  <si>
+    <t>BCC or BRA</t>
+  </si>
+  <si>
+    <t>MOVE FM CCR</t>
+  </si>
+  <si>
+    <t>MOVE FM Sr</t>
   </si>
 </sst>
 </file>
@@ -333,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -350,11 +380,21 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -362,6 +402,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G28" totalsRowShown="0">
+  <autoFilter ref="A1:G28"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="OP MODE"/>
+    <tableColumn id="2" name="VALUE"/>
+    <tableColumn id="3" name="Hex value" dataDxfId="1"/>
+    <tableColumn id="4" name="1's to End Range"/>
+    <tableColumn id="5" name="Invalid sizes" dataDxfId="0"/>
+    <tableColumn id="6" name="Invalid EA Mode"/>
+    <tableColumn id="7" name="Invalid Reg"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,19 +707,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
@@ -676,19 +732,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>23</v>
       </c>
       <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -699,10 +755,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2">
         <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -713,19 +772,19 @@
         <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>29</v>
+      <c r="E3" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -733,22 +792,22 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -756,22 +815,22 @@
         <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -779,22 +838,22 @@
         <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -802,22 +861,22 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -825,19 +884,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>44</v>
+      <c r="E8" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -845,22 +904,22 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D9">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
-        <v>35</v>
+      <c r="E9" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -868,19 +927,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>111</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -888,19 +947,19 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -908,19 +967,22 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
+      <c r="E12" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -928,19 +990,22 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D13">
         <v>4</v>
       </c>
+      <c r="E13" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -948,19 +1013,22 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
+      <c r="E14" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -968,16 +1036,19 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D15">
         <v>4</v>
       </c>
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -985,22 +1056,22 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1008,7 +1079,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="5">
         <v>4400</v>
@@ -1016,14 +1087,14 @@
       <c r="D17">
         <v>3</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="5">
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1031,22 +1102,22 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
-      <c r="E18" t="s">
-        <v>59</v>
+      <c r="E18" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1054,22 +1125,22 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D19">
         <v>4</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="5">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1077,22 +1148,22 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D20">
         <v>4</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="5">
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1100,22 +1171,22 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="5">
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1123,80 +1194,85 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
+      <c r="E22" s="5"/>
       <c r="F22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4" t="s">
-        <v>74</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
+      <c r="E24" s="8" t="s">
+        <v>92</v>
+      </c>
       <c r="F24" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
       <c r="C25" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="5">
         <v>11</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1204,7 +1280,7 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C26" s="5">
         <v>6000</v>
@@ -1212,14 +1288,14 @@
       <c r="D26">
         <v>3</v>
       </c>
-      <c r="E26" t="s">
-        <v>65</v>
+      <c r="E26" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="F26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1227,7 +1303,7 @@
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="5">
         <v>6000</v>
@@ -1235,14 +1311,14 @@
       <c r="D27">
         <v>7</v>
       </c>
-      <c r="E27" t="s">
-        <v>65</v>
+      <c r="E27" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1250,50 +1326,241 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" t="s">
-        <v>65</v>
+      <c r="E28" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="F28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="5">
+        <v>8800000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="5">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="5">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="5">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="5">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="6" t="s">
+      <c r="B44" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="5">
+        <v>4880</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="5">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" s="5">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="5">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>19</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D29">
-        <v>16</v>
-      </c>
-      <c r="E29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" t="s">
-        <v>65</v>
-      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added support for more OP
</commit_message>
<xml_diff>
--- a/Raw Data/OP Code Datasheet.xlsx
+++ b/Raw Data/OP Code Datasheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="112">
   <si>
     <t>OP MODE</t>
   </si>
@@ -328,6 +328,30 @@
   </si>
   <si>
     <t>MOVE FM Sr</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>ADDA</t>
+  </si>
+  <si>
+    <t>0100111001110001</t>
+  </si>
+  <si>
+    <t>1101XXXXXX</t>
+  </si>
+  <si>
+    <t>D000</t>
+  </si>
+  <si>
+    <t>4E71</t>
+  </si>
+  <si>
+    <t>ADD/ADDA</t>
   </si>
 </sst>
 </file>
@@ -405,8 +429,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G28" totalsRowShown="0">
-  <autoFilter ref="A1:G28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G31" totalsRowShown="0">
+  <autoFilter ref="A1:G31"/>
   <tableColumns count="7">
     <tableColumn id="1" name="OP MODE"/>
     <tableColumn id="2" name="VALUE"/>
@@ -707,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1344,216 +1368,262 @@
         <v>63</v>
       </c>
     </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="5"/>
+    </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>95</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="B30" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="5">
-        <v>8800000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>86</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>87</v>
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>80</v>
+        <v>64</v>
+      </c>
+      <c r="B36" s="5">
+        <v>8800000</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>84</v>
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="5">
-        <v>9000</v>
+        <v>96</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>100</v>
-      </c>
-      <c r="B40" s="5">
-        <v>8000</v>
+        <v>98</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" s="5">
-        <v>6000</v>
+        <v>9</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="5">
-        <v>5100</v>
+        <v>99</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>91</v>
+        <v>7</v>
+      </c>
+      <c r="B43" s="5">
+        <v>9000</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>38</v>
+        <v>10</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="B45" s="5">
-        <v>4880</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="B46" s="5">
-        <v>4400</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>11</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>82</v>
+        <v>8</v>
+      </c>
+      <c r="B47" s="5">
+        <v>5100</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>75</v>
+        <v>22</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="5">
-        <v>1140</v>
+        <v>3</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>102</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>49</v>
+        <v>104</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="B51" s="5">
-        <v>1030</v>
+        <v>4880</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>67</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>89</v>
+        <v>14</v>
+      </c>
+      <c r="B52" s="5">
+        <v>4400</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>19</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>88</v>
+        <v>11</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>76</v>
+        <v>24</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="5">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B61" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="5"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>